<commit_message>
VSCode live debugging now working, exporting chart, and removing current files data to replace it
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -2,11 +2,11 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <bookViews>
-    <workbookView/>
+    <workbookView activeTab="-1"/>
   </bookViews>
   <sheets>
-    <sheet name="Chart" sheetId="1" r:id="rId1"/>
-    <sheet name="Data_Cells" sheetId="2" r:id="rId2"/>
+    <sheet name="Chart" sheetId="1" r:id="rId4"/>
+    <sheet name="Data_Cells" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
@@ -74,6 +74,123 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <ser xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>
+              </c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Chart'!A10</c:f>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chart'!A5</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </ser>
+        <c:smooth val="0"/>
+        <c:axId val="1"/>
+        <c:axId val="2"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <graphicFrame xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name="Cool Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
@@ -82,6 +199,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
working example of charting
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -77,11 +77,15 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:chart>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:rotY val="20"/>
+      <c:perspective val="30"/>
+    </c:view3D>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
         <ser xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -94,52 +98,18 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Chart'!A10</c:f>
+              <c:f>'Chart'!$A$1:$J$1</c:f>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Chart'!A5</c:f>
+              <c:f>'Data_Cells'!$A$2:$J$2</c:f>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </ser>
-        <c:smooth val="0"/>
-        <c:axId val="1"/>
-        <c:axId val="2"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="1"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
+      </c:pie3DChart>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>

</xml_diff>

<commit_message>
adding row and headers, not charting
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -13,7 +13,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>PositionId</t>
+  </si>
+  <si>
+    <t>CompanyId</t>
+  </si>
+  <si>
+    <t>CandidateId</t>
+  </si>
+  <si>
+    <t>PositionName</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>EndDate</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>MinSalary</t>
+  </si>
+  <si>
+    <t>MaxSalary</t>
+  </si>
   <si>
     <t>Test Position One</t>
   </si>
@@ -100,12 +130,150 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'Chart'!$A$1:$J$1</c:f>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Data_Cells'!$A$2:$J$2</c:f>
+              <c:f>'Chart'!</c:f>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chart'!B1:J1</c:f>
+            </c:numRef>
+          </c:val>
+        </ser>
+        <ser xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>
+              </c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Chart'!</c:f>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chart'!B2:J2</c:f>
+            </c:numRef>
+          </c:val>
+        </ser>
+        <ser xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>
+              </c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Chart'!</c:f>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chart'!B3:J3</c:f>
+            </c:numRef>
+          </c:val>
+        </ser>
+        <ser xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>
+              </c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Chart'!</c:f>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chart'!B4:J4</c:f>
+            </c:numRef>
+          </c:val>
+        </ser>
+        <ser xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>
+              </c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Chart'!</c:f>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chart'!B5:J5</c:f>
+            </c:numRef>
+          </c:val>
+        </ser>
+        <ser xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>
+              </c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Chart'!</c:f>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chart'!B6:J6</c:f>
+            </c:numRef>
+          </c:val>
+        </ser>
+        <ser xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>
+              </c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Chart'!</c:f>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chart'!B7:J7</c:f>
             </c:numRef>
           </c:val>
         </ser>
@@ -175,47 +343,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0">
-        <v>1123456</v>
-      </c>
-      <c r="B1" s="0">
-        <v>2123456</v>
-      </c>
-      <c r="C1" s="0">
-        <v>3123456</v>
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="0">
-        <v>43466</v>
-      </c>
-      <c r="G1" s="0">
-        <v>43467</v>
-      </c>
-      <c r="H1" s="0">
-        <v>0</v>
-      </c>
-      <c r="I1" s="0">
-        <v>60000</v>
-      </c>
-      <c r="J1" s="0">
-        <v>70000</v>
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>2123456</v>
+        <v>1123456</v>
       </c>
       <c r="B2" s="0">
         <v>2123456</v>
@@ -224,16 +392,16 @@
         <v>3123456</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F2" s="0">
+        <v>43466</v>
+      </c>
+      <c r="G2" s="0">
         <v>43467</v>
-      </c>
-      <c r="G2" s="0">
-        <v>43468</v>
       </c>
       <c r="H2" s="0">
         <v>0</v>
@@ -247,25 +415,25 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>3123456</v>
+        <v>2123456</v>
       </c>
       <c r="B3" s="0">
-        <v>32123456</v>
+        <v>2123456</v>
       </c>
       <c r="C3" s="0">
         <v>3123456</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F3" s="0">
+        <v>43467</v>
+      </c>
+      <c r="G3" s="0">
         <v>43468</v>
-      </c>
-      <c r="G3" s="0">
-        <v>43469</v>
       </c>
       <c r="H3" s="0">
         <v>0</v>
@@ -279,25 +447,25 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>4123456</v>
+        <v>3123456</v>
       </c>
       <c r="B4" s="0">
-        <v>4123456</v>
+        <v>32123456</v>
       </c>
       <c r="C4" s="0">
         <v>3123456</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="F4" s="0">
+        <v>43468</v>
+      </c>
+      <c r="G4" s="0">
         <v>43469</v>
-      </c>
-      <c r="G4" s="0">
-        <v>43470</v>
       </c>
       <c r="H4" s="0">
         <v>0</v>
@@ -311,25 +479,25 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>123456</v>
+        <v>4123456</v>
       </c>
       <c r="B5" s="0">
-        <v>2123456</v>
+        <v>4123456</v>
       </c>
       <c r="C5" s="0">
         <v>3123456</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F5" s="0">
-        <v>43471</v>
+        <v>43469</v>
       </c>
       <c r="G5" s="0">
-        <v>43472</v>
+        <v>43470</v>
       </c>
       <c r="H5" s="0">
         <v>0</v>
@@ -338,6 +506,38 @@
         <v>60000</v>
       </c>
       <c r="J5" s="0">
+        <v>70000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>123456</v>
+      </c>
+      <c r="B6" s="0">
+        <v>2123456</v>
+      </c>
+      <c r="C6" s="0">
+        <v>3123456</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="0">
+        <v>43471</v>
+      </c>
+      <c r="G6" s="0">
+        <v>43472</v>
+      </c>
+      <c r="H6" s="0">
+        <v>0</v>
+      </c>
+      <c r="I6" s="0">
+        <v>60000</v>
+      </c>
+      <c r="J6" s="0">
         <v>70000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finished fixing the various formats of charts
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -107,6 +107,25 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr/>
+              <a:t>Test Chart 0</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:view3D>
       <c:rotX val="30"/>
       <c:rotY val="20"/>
@@ -130,150 +149,12 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'Chart'!</c:f>
+              <c:f>=Data_Cells!$A$1:$J$1</c:f>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Chart'!B1:J1</c:f>
-            </c:numRef>
-          </c:val>
-        </ser>
-        <ser xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>
-              </c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Chart'!</c:f>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Chart'!B2:J2</c:f>
-            </c:numRef>
-          </c:val>
-        </ser>
-        <ser xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>
-              </c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Chart'!</c:f>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Chart'!B3:J3</c:f>
-            </c:numRef>
-          </c:val>
-        </ser>
-        <ser xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>
-              </c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Chart'!</c:f>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Chart'!B4:J4</c:f>
-            </c:numRef>
-          </c:val>
-        </ser>
-        <ser xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>
-              </c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Chart'!</c:f>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Chart'!B5:J5</c:f>
-            </c:numRef>
-          </c:val>
-        </ser>
-        <ser xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>
-              </c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Chart'!</c:f>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Chart'!B6:J6</c:f>
-            </c:numRef>
-          </c:val>
-        </ser>
-        <ser xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>
-              </c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Chart'!</c:f>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Chart'!B7:J7</c:f>
+              <c:f>=Data_Cells!$A$2:$J$6</c:f>
             </c:numRef>
           </c:val>
         </ser>
@@ -294,6 +175,244 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr/>
+              <a:t>Test Chart 1</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:rotY val="20"/>
+      <c:perspective val="30"/>
+    </c:view3D>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <ser xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>
+              </c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data_Cells!$A$1:$J$1</c:f>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>=Data_Cells!$A$2:$J$6</c:f>
+            </c:numRef>
+          </c:val>
+        </ser>
+      </c:pie3DChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr/>
+              <a:t>Test Chart 2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <ser xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>
+              </c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data_Cells!$A$1:$J$1</c:f>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>=Data_Cells!$A$2:$J$6</c:f>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </ser>
+        <c:axId val="1"/>
+        <c:axId val="2"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr/>
+              <a:t>Test Chart 3</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:doughnutChart>
+        <c:varyColors val="1"/>
+        <ser xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>
+              </c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data_Cells!$A$1:$J$1</c:f>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>=Data_Cells!$A$2:$J$6</c:f>
+            </c:numRef>
+          </c:val>
+        </ser>
+        <c:firstSliceAng val="0"/>
+        <c:holeSize val="50"/>
+      </c:doughnutChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -304,14 +423,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <graphicFrame xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1" name="Cool Chart"/>
+        <xdr:cNvPr id="4" name="chartZero"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -326,6 +445,96 @@
     </graphicFrame>
     <clientData xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <graphicFrame xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="chartOne"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <graphicFrame xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="chartTwo"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <graphicFrame xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="chartThree"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 

</xml_diff>

<commit_message>
final chart model for json
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -3,18 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="-1"/>
   </bookViews>
   <sheets>
-    <sheet name="Chart" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Data_Cells" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Chart" sheetId="1" r:id="rId6"/>
+    <sheet name="Data_Cells" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>PositionId</t>
   </si>
@@ -46,39 +46,34 @@
     <t>MaxSalary</t>
   </si>
   <si>
-    <t xml:space="preserve">Test Position One</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description One</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Position Two</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description Two</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Position Three</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description Three</t>
-  </si>
-  <si>
-    <t>Junk</t>
-  </si>
-  <si>
-    <t>junk</t>
+    <t>Test Position One</t>
+  </si>
+  <si>
+    <t>Description One</t>
+  </si>
+  <si>
+    <t>Test Position Two</t>
+  </si>
+  <si>
+    <t>Description Two</t>
+  </si>
+  <si>
+    <t>Test Position Three</t>
+  </si>
+  <si>
+    <t>Description Three</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -100,10 +95,10 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -114,17 +109,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
-  <c:date1904 val="0"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:chart>
     <c:title>
       <c:tx>
@@ -139,14 +124,12 @@
               <a:rPr/>
               <a:t>Test Chart 0</a:t>
             </a:r>
-            <a:endParaRPr/>
           </a:p>
         </c:rich>
       </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:view3D>
       <c:rotX val="30"/>
       <c:rotY val="20"/>
@@ -156,12 +139,35 @@
       <c:layout/>
       <c:pie3DChart>
         <c:varyColors val="1"/>
-        <c:ser>
+        <ser xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f xml:space="preserve">
+              <c:f>
+              </c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>=Data_Cells!$A$1:$J$1</c:f>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>=Data_Cells!$A$2:$J$10</c:f>
+            </c:numRef>
+          </c:val>
+        </ser>
+        <ser xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>
               </c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -178,15 +184,7 @@
               <c:f>=Data_Cells!$A$2:$J$6</c:f>
             </c:numRef>
           </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showBubbleSize val="0"/>
-          <c:showCatName val="0"/>
-          <c:showLegendKey val="0"/>
-          <c:showPercent val="0"/>
-          <c:showSerName val="0"/>
-          <c:showVal val="0"/>
-        </c:dLbls>
+        </ser>
       </c:pie3DChart>
     </c:plotArea>
     <c:legend>
@@ -195,34 +193,17 @@
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:spPr bwMode="auto">
-    <a:xfrm>
-      <a:off x="0" y="0"/>
-      <a:ext cx="0" cy="0"/>
-    </a:xfrm>
-  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins l="0.69999999999999996" r="0.69999999999999996" t="0.75" b="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
-  <c:date1904 val="0"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:chart>
     <c:title>
       <c:tx>
@@ -237,14 +218,12 @@
               <a:rPr/>
               <a:t>Test Chart 1</a:t>
             </a:r>
-            <a:endParaRPr/>
           </a:p>
         </c:rich>
       </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:view3D>
       <c:rotX val="30"/>
       <c:rotY val="20"/>
@@ -254,12 +233,12 @@
       <c:layout/>
       <c:pie3DChart>
         <c:varyColors val="1"/>
-        <c:ser>
+        <ser xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f xml:space="preserve">
+              <c:f>
               </c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -277,15 +256,7 @@
               <c:f>=Data_Cells!$A$2:$J$6</c:f>
             </c:numRef>
           </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showBubbleSize val="0"/>
-          <c:showCatName val="0"/>
-          <c:showLegendKey val="0"/>
-          <c:showPercent val="0"/>
-          <c:showSerName val="0"/>
-          <c:showVal val="0"/>
-        </c:dLbls>
+        </ser>
       </c:pie3DChart>
     </c:plotArea>
     <c:legend>
@@ -294,34 +265,17 @@
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:spPr bwMode="auto">
-    <a:xfrm>
-      <a:off x="0" y="0"/>
-      <a:ext cx="0" cy="0"/>
-    </a:xfrm>
-  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins l="0.69999999999999996" r="0.69999999999999996" t="0.75" b="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
-  <c:date1904 val="0"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:chart>
     <c:title>
       <c:tx>
@@ -336,25 +290,23 @@
               <a:rPr/>
               <a:t>Test Chart 2</a:t>
             </a:r>
-            <a:endParaRPr/>
           </a:p>
         </c:rich>
       </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
-        <c:ser>
+        <ser xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f xml:space="preserve">
+              <c:f>
               </c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -375,15 +327,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showBubbleSize val="0"/>
-          <c:showCatName val="0"/>
-          <c:showLegendKey val="0"/>
-          <c:showPercent val="0"/>
-          <c:showSerName val="0"/>
-          <c:showVal val="0"/>
-        </c:dLbls>
+        </ser>
         <c:axId val="1"/>
         <c:axId val="2"/>
       </c:scatterChart>
@@ -394,12 +338,9 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="2"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="2"/>
@@ -408,11 +349,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr bwMode="auto"/>
-        </c:majorGridlines>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
+        <c:majorGridlines/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1"/>
         <c:crosses val="autoZero"/>
@@ -425,34 +362,17 @@
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:spPr bwMode="auto">
-    <a:xfrm>
-      <a:off x="0" y="0"/>
-      <a:ext cx="0" cy="0"/>
-    </a:xfrm>
-  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins l="0.69999999999999996" r="0.69999999999999996" t="0.75" b="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
-  <c:date1904 val="0"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:chart>
     <c:title>
       <c:tx>
@@ -467,24 +387,22 @@
               <a:rPr/>
               <a:t>Test Chart 3</a:t>
             </a:r>
-            <a:endParaRPr/>
           </a:p>
         </c:rich>
       </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:doughnutChart>
         <c:varyColors val="1"/>
-        <c:ser>
+        <ser xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f xml:space="preserve">
+              <c:f>
               </c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -502,15 +420,7 @@
               <c:f>=Data_Cells!$A$2:$J$6</c:f>
             </c:numRef>
           </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showBubbleSize val="0"/>
-          <c:showCatName val="0"/>
-          <c:showLegendKey val="0"/>
-          <c:showPercent val="0"/>
-          <c:showSerName val="0"/>
-          <c:showVal val="0"/>
-        </c:dLbls>
+        </ser>
         <c:firstSliceAng val="0"/>
         <c:holeSize val="50"/>
       </c:doughnutChart>
@@ -521,25 +431,18 @@
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:spPr bwMode="auto">
-    <a:xfrm>
-      <a:off x="0" y="0"/>
-      <a:ext cx="0" cy="0"/>
-    </a:xfrm>
-  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins l="0.69999999999999996" r="0.69999999999999996" t="0.75" b="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -552,12 +455,10 @@
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <graphicFrame xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="chartZero" hidden="0"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvPr id="4" name="chartZero"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -568,10 +469,10 @@
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
+    </graphicFrame>
+    <clientData xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -584,12 +485,10 @@
       <xdr:row>43</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <graphicFrame xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="chartOne" hidden="0"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvPr id="5" name="chartOne"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -600,10 +499,10 @@
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
+    </graphicFrame>
+    <clientData xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -616,12 +515,10 @@
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <graphicFrame xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="chartTwo" hidden="0"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvPr id="6" name="chartTwo"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -632,10 +529,10 @@
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
+    </graphicFrame>
+    <clientData xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -648,12 +545,10 @@
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <graphicFrame xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="chartThree" hidden="0"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvPr id="7" name="chartThree"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -664,8 +559,8 @@
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
+    </graphicFrame>
+    <clientData xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
@@ -1077,27 +972,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <printOptions headings="0" gridLines="0" gridLinesSet="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -1293,41 +1183,7 @@
         <v>70000</v>
       </c>
     </row>
-    <row ht="15" r="7">
-      <c r="A7" s="0">
-        <v>342342</v>
-      </c>
-      <c r="B7" s="0">
-        <v>43242</v>
-      </c>
-      <c r="C7" s="0">
-        <v>43234</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="0">
-        <v>344</v>
-      </c>
-      <c r="G7" s="0">
-        <v>4342</v>
-      </c>
-      <c r="H7" s="0">
-        <v>434</v>
-      </c>
-      <c r="I7" s="0">
-        <v>4342</v>
-      </c>
-      <c r="J7" s="0">
-        <v>4343</v>
-      </c>
-    </row>
   </sheetData>
-  <printOptions headings="0" gridLines="0" gridLinesSet="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>